<commit_message>
change bug and add newsbrowse table
</commit_message>
<xml_diff>
--- a/NewsRec/z-others/data/original/1-国际要闻国际频道光明网.xlsx
+++ b/NewsRec/z-others/data/original/1-国际要闻国际频道光明网.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\推荐系统\3-数据集\新闻推荐实例数据\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\NewsRecSys\NewsRec\z-others\data\original\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="287">
   <si>
     <t>标题</t>
   </si>
@@ -549,18 +549,6 @@
     <t>德国政府将投入15亿欧元以改善城市空气质量</t>
   </si>
   <si>
-    <t>2018-12-04 09:38</t>
-  </si>
-  <si>
-    <t>　　中新社柏林12月3日(记者彭大伟)德国总理默克尔3日宣布，德联邦政府决定将其用于改善各地城市空气质量的资金从此前的10亿欧元增加至15亿欧元。
-　　默克尔当天在柏林与各州代表围绕城市空气质量议题举行了会谈。会谈结束后，默克尔宣布了上述决定。她表示，除将去年宣布的10亿欧元“清洁空气应急计划”资金增加至15亿外，德国联邦政府还将支出约4.3亿欧元，用于推动地方层面实施汽车硬件升级。
-　　自从2015年德国汽车厂商曝出“尾气门”事件以来，柴油车的存废在德国持续成为热门话题。截至目前，包括首都柏林和经济发达的汉堡、科隆等城市行政法院都在裁决中要求未来在部分路段实施柴油车禁行。尽管离正式实施仍有一段时日，但由于德国汽车巨头和工会等已对“一刀切”的禁柴令表达了强烈反对，德国政府推出的前述方案被外界解读为试图在环保和各方利益之间寻求折中。
-　　截至目前，围绕这一议题，默克尔已邀请地方各州代表在柏林举行了三次会议。德国政府在文告中表示，3日会议的焦点是如何解决“一方面需要可持续地改善空气质量，另一方面要确保公民出行便利”这一挑战。德国政府称，联邦和地方的共同目标是控制污染极限值，同时尽可能地避免最终实施“禁柴令”。
-　　默克尔3日当天表示，政府正在高负荷地落实汽车硬件升级所需的先决条件。德国联邦交通部长朔伊尔则更为直接地表示，联邦政府正在用一切手段避免“禁柴”成为现实，并给予地方巨大的支持，“我们的目标是，既要避免禁行，也要提供解决方案。”
-　　为实现上述目标，德国联邦政府去年推出了“清洁空气应急计划”，其旨在从2017年至2020年间通过资助城市电动交通、交通系统数字化、柴油公交车改造等措施改善城市空气质量。
-　　德国政府表示，上述计划加上此前已开展的汽车软件升级两方面措施实施以来，德国出现空气质量“爆表”(突破污染极限值)的城市数已从2016年的90个下降至2017年的65个。[责编：张倩]</t>
-  </si>
-  <si>
     <t>英国工党欲借“脱欧”协议表决逼首相下台</t>
   </si>
   <si>
@@ -1087,14 +1075,6 @@
     <t>2018-12-03 10:13</t>
   </si>
   <si>
-    <t>　　中新网12月3日电据外媒报道，当地时间2日，联合国气候峰会在波兰卡托维兹揭幕，全球约200个国家代表将在未来两周商讨如何落实2015《巴黎协定》。东道主波兰将推动与会各国共同发表宣言，承诺逐步淘汰化石燃料，减少温室气体排放。
-　　资料图：2017年11月6日，联合国气候变化框架公约第23次缔约方大会在德国波恩开幕。图为开幕式现场。中新社记者 彭大伟摄
-　　报道称，全球180多个国家已确认《巴黎协定》，但近年部分国家面对国内压力，放宽碳排放限制，各方视这次会议为各国展示减排决心的机会。
-　　会议重点包括制定记录温室气体排放量的机制，以及各国的减排措施，还会讨论在2020年整合数据，计算出全球总排放量，并为贫穷国家提供财政支援，应对气候变化威胁。
-　　以往联合国气候峰会的主席国，在此次会议前罕见的发表了共同声明，呼吁各国采取“决定性行动”，应对迫在眉睫的威胁，“气候变化的动向日益加剧，我们的经济和社会需要深层演变”。
-　　美国此前已宣布退出该协定。《联合国气候变化框架公约》(UNFCCC)前秘书长菲盖尔批评美国退出协定的举动，“美国日益感受到气候变化的冲击，但仍继续拒绝聆听科学的客观声音。”[责编：王宏泽]</t>
-  </si>
-  <si>
     <t>乌指俄军在边境集结 欧洲国家吁普京缓和俄乌局势</t>
   </si>
   <si>
@@ -1156,65 +1136,6 @@
     <t>默克尔接班人之战现“两强争霸” 胜负难料</t>
   </si>
   <si>
-    <t>2018-12-03 09:04</t>
-  </si>
-  <si>
-    <t>　　德国总理安格拉·默克尔所属基督教民主联盟（基民盟）定于7日选举新主席。随着选举进入倒计时，“两强”候选人弗里德里希·默茨和安妮格雷特·克兰普·卡伦鲍尔加大攻势，向党主席发起冲刺。
-　　一些政治分析师说，从民意调查结果看，两人所获支持率不相上下，选战将相当激烈。
-　　【发起对攻】
-　　基民盟定于7日至8日在汉堡举行全国党代会，选举新任党主席。按照基民盟传统，党主席与联邦总理通常由同一人出任。这场选举的胜者将成为默克尔“接班人”，有望出任下任联邦政府总理。
-　　三名主要候选人分别是默克尔的“老对手”默茨、有“小默克尔”之称的基民盟秘书长卡伦鲍尔和卫生部长延斯·施潘。
-　　最近一个月，基民盟在各地举办8场推介会，由上述候选人向基层党员介绍竞选主张。随着选举日期临近，“两强”候选人默茨和卡伦鲍尔进入对攻模式，提出完全不同的主张。
-　　默茨11月30日在柏林推介会上说，如果他当选党主席，基民盟“毫无疑问将把国内安全放在首位”。他承诺，将逆转基民盟支持率下跌的颓势，力争重新获得保守派政党支持。
-　　卡伦鲍尔把矛头指向默茨的商界背景。默茨上月自曝年薪大约100万欧元（约合787万元人民币），被指属于“上流社会”、不接地气。卡伦鲍尔说：“我不确定成为百万富翁是真正的人生目标。”
-　　这名女性候选人认为，要增加基民盟吸引力，应停止攻击对手，加大自身宣传力度。
-　　【胜负难料】
-　　默克尔“接班人”之战打响初期，默茨在多项民调中处于领跑状态。随着选举进入倒计时，卡伦鲍尔所获支持率不断攀升，反超默茨。
-　　德国电视一台11月29日发布一项民调，显示所有调查对象中，39%支持卡伦鲍尔接替默克尔出任基民盟主席。基民盟成员中，48%的人支持卡伦鲍尔。同一项民调中，默茨在所有调查对象中所获支持率为26%，在基民盟成员中支持率为35%。
-　　一些政治分析师判断，卡伦鲍尔和默茨各具优势，选战将相当激烈。
-　　路透社报道，参加投票的基民盟党员中，大多数为议员、市长等政界人士，对卡伦鲍尔有利，阔别政坛近10年的默茨处于劣势。不过，投票者中近30%来自默茨家乡所在州，默茨可以打“老乡牌”拉票。
-　　卡伦鲍尔现年56岁，是默克尔的亲密盟友，据信是后者“中意”的继任人选。默克尔对她的欣赏溢于言表。今年2月，默克尔宣布提名卡伦鲍尔出任基民盟秘书长，一时口误，称后者有望成为“基民盟有史以来第一名女秘书长”，忘了自己才是这项纪录的创造者。（张旌）（新华社专特稿）
-[责编：袁晴]</t>
-  </si>
-  <si>
-    <t>2018-12-03 09:03</t>
-  </si>
-  <si>
-    <t>　　乌克兰总统彼得罗·波罗申科指认俄罗斯陆军及其武器装备正在乌俄边境集结。
-　　借出席二十国集团(G20)领导人第十三次峰会之机，法国、德国等欧洲国家领导人呼吁俄罗斯总统弗拉基米尔·普京为缓和俄乌紧张局势采取措施。
-　　【说“强敌”】
-　　乌克兰总统波罗申科1日在一场军事活动上说，俄罗斯已经在乌俄边境部署超过8000名士兵、1400件火炮或多管火箭发射系统、900辆坦克、2300辆装甲战车、500架飞机和300架直升机。
-　　他说，俄罗斯正在增加海上兵力部署。“在黑海、亚速海和爱琴海，（俄方）超过80艘舰船和8艘潜水艇正在巡逻。”
-　　美联社报道，无法证实波罗申科所述俄方部署的规模。
-　　乌克兰官员指责俄方于11月25日在刻赤海峡拦截和扣留乌方海军3艘船只后“实际”封锁乌方在亚速海的两个主要港口。
-　　波罗申科说，俄罗斯正在观察国际社会是否会允许俄方声称亚速海和黑海是俄罗斯领海，称“克里姆林宫正进一步试探全球秩序的力量。”
-　　11月25日的事件后，波罗申科说服最高拉达、即乌克兰议会通过戒严令，拒绝16岁至60岁俄方男性公民入境乌克兰。乌方边境管理部门12月1日说，自限制入境令11月30日生效以来，已有大约100名俄方男性公民尝试入境但遭到拒绝。
-　　【借“外力”】
-　　美联社报道，欧洲国家领导人接连指责俄罗斯扣留乌方船只，七国集团(G7)外交部长发表声明，要求俄方释放乌方船员。
-　　法国总统埃马纽埃尔·马克龙11月30日与普京会晤。法新社以一名法方官员为消息源报道，马克龙向普京施压，要求俄方“采取必要举措，以缓和局势”。
-　　德国总理安格拉·默克尔12月1日与普京共进早餐，谈及刻赤海峡冲突。她要求俄方避免局势恶化，“必须确保驶向乌克兰海岸和城市的船只在亚速海自由通行”。
-　　美国方面，总统唐纳德·特朗普原定在G20峰会期间与普京会晤，却以刻赤海峡冲突致使美俄元首不宜举行会晤为由予以取消。峰会期间，特朗普见了普京，只是把会晤简化为“简短交谈”。
-　　按照普京的说法，就刻赤海峡冲突，他与特朗普交换了看法，双方没有达成共识。
-　　【没“讨论”】
-　　普京12月1日在G20峰会期间一场记者会上说，俄方没有与乌方讨论释放24名船员的可能性。
-　　他没有回避西方国家就刻赤海峡冲突对俄方的指责。
-　　谈及美方取消双边会晤，普京说特朗普取消与他的正式会晤“太糟糕”，暗示两国元首没有充分交换意见的机会可能导致不良后果。
-　　普京说：“我回答了他（特朗普）有关黑海发生事件的问题。他有他的看法，我有我的。我们坚持各自立场。”
-　　美联社报道，俄方认为，美方取消正式会晤是为了回避国内对特朗普涉嫌与俄罗斯方面在2016年总统选举中“串通”的指认。普京在记者会上的说法是：“打俄罗斯牌已经成为解决美国国内政治问题的便利工具。”
-　　普京与马克龙会面时“仔细画出乌克兰海岸线的地图”，以解释俄方扣留乌方船只“合法”。
-　　俄方认定乌方船只没有获得进入俄方领海的许可，24名船员“非法越境”。乌方则指认俄方舰艇故意撞船并开火伤人。（包雪琳）（新华社专特稿）
-[责编：袁晴]</t>
-  </si>
-  <si>
-    <t>　　新华社华盛顿１２月２日电（记者刘品然　朱东阳）美国总统特朗普１日晚对媒体表示，他或将于明年１月或２月与朝鲜最高领导人金正恩再次举行会晤。
-　　据白宫２日发布的消息，特朗普１日晚从阿根廷乘飞机返回美国途中对媒体说，他与金正恩有着“非常好的关系”，并认为两人或将于明年１月或２月举行会晤。
-　　特朗普表示，目前还没有确定会晤地点，有３个可能的地点正在考虑中。
-　　他还说，会在未来某个时刻邀请金正恩访问美国。
-　　特朗普此前曾表示，他与金正恩的第二次会晤将在今年１１月６日美国中期选举后举行。美国媒体１０月下旬曾援引匿名白宫官员的话报道说，特朗普与金正恩的第二次会晤可能会在明年年初举行。
-　　今年６月，特朗普与金正恩在新加坡会晤并签署联合声明，就“建立新的朝美关系”以及“构建朝鲜半岛持久稳定和平机制”达成一致。
-[责编：袁晴]</t>
-  </si>
-  <si>
     <t>老布什国葬5日举行 生前最后一句话“我也爱你”</t>
   </si>
   <si>
@@ -1286,34 +1207,6 @@
 　　警方宣称，暴力行动是由极右及极左分子引发，不过卡斯塔内称，大部分被捕人士都是受到激进组织煽动的一般示威者。司法部消息人士透露，继巴黎骚乱后，南部城市纳博讷有示威者闯入高速公路，并焚烧一个收费亭，里昂附近连接法国东南部及东北部的A6高速公路，亦遭示威者堵塞。[责编：程雪]</t>
   </si>
   <si>
-    <t>2018-12-03 08:32</t>
-  </si>
-  <si>
-    <t>　　乌克兰总统彼得罗·波罗申科指认俄罗斯陆军及其武器装备正在乌俄边境集结。
-　　借出席二十国集团(G20)领导人第十三次峰会之机，法国、德国等欧洲国家领导人呼吁俄罗斯总统弗拉基米尔·普京为缓和俄乌紧张局势采取措施。
-　　【说“强敌”】
-　　乌克兰总统波罗申科1日在一场军事活动上说，俄罗斯已经在乌俄边境部署超过8000名士兵、1400件火炮或多管火箭发射系统、900辆坦克、2300辆装甲战车、500架飞机和300架直升机。
-　　他说，俄罗斯正在增加海上兵力部署。“在黑海、亚速海和爱琴海，（俄方）超过80艘舰船和8艘潜水艇正在巡逻。”
-　　美联社报道，无法证实波罗申科所述俄方部署的规模。
-　　乌克兰官员指责俄方于11月25日在刻赤海峡拦截和扣留乌方海军3艘船只后“实际”封锁乌方在亚速海的两个主要港口。
-　　波罗申科说，俄罗斯正在观察国际社会是否会允许俄方声称亚速海和黑海是俄罗斯领海，称“克里姆林宫正进一步试探全球秩序的力量。”
-　　11月25日的事件后，波罗申科说服最高拉达、即乌克兰议会通过戒严令，拒绝16岁至60岁俄方男性公民入境乌克兰。乌方边境管理部门12月1日说，自限制入境令11月30日生效以来，已有大约100名俄方男性公民尝试入境但遭到拒绝。
-　　【借“外力”】
-　　美联社报道，欧洲国家领导人接连指责俄罗斯扣留乌方船只，七国集团(G7)外交部长发表声明，要求俄方释放乌方船员。
-　　法国总统埃马纽埃尔·马克龙11月30日与普京会晤。法新社以一名法方官员为消息源报道，马克龙向普京施压，要求俄方“采取必要举措，以缓和局势”。
-　　德国总理安格拉·默克尔12月1日与普京共进早餐，谈及刻赤海峡冲突。她要求俄方避免局势恶化，“必须确保驶向乌克兰海岸和城市的船只在亚速海自由通行”。
-　　美国方面，总统唐纳德·特朗普原定在G20峰会期间与普京会晤，却以刻赤海峡冲突致使美俄元首不宜举行会晤为由予以取消。峰会期间，特朗普见了普京，只是把会晤简化为“简短交谈”。
-　　按照普京的说法，就刻赤海峡冲突，他与特朗普交换了看法，双方没有达成共识。
-　　【没“讨论”】
-　　普京12月1日在G20峰会期间一场记者会上说，俄方没有与乌方讨论释放24名船员的可能性。
-　　他没有回避西方国家就刻赤海峡冲突对俄方的指责。
-　　谈及美方取消双边会晤，普京说特朗普取消与他的正式会晤“太糟糕”，暗示两国元首没有充分交换意见的机会可能导致不良后果。
-　　普京说：“我回答了他（特朗普）有关黑海发生事件的问题。他有他的看法，我有我的。我们坚持各自立场。”
-　　美联社报道，俄方认为，美方取消正式会晤是为了回避国内对特朗普涉嫌与俄罗斯方面在2016年总统选举中“串通”的指认。普京在记者会上的说法是：“打俄罗斯牌已经成为解决美国国内政治问题的便利工具。”
-　　普京与马克龙会面时“仔细画出乌克兰海岸线的地图”，以解释俄方扣留乌方船只“合法”。
-　　俄方认定乌方船只没有获得进入俄方领海的许可，24名船员“非法越境”。乌方则指认俄方舰艇故意撞船并开火伤人。（包雪琳）（新华社专特稿）[责编：程雪]</t>
-  </si>
-  <si>
     <t>洛佩斯就任墨西哥新总统 誓言让墨西哥“重生”</t>
   </si>
   <si>
@@ -1404,14 +1297,6 @@
 　　本次大会的高级别会议将于３日开始举行，联合国秘书长古特雷斯、波兰总统杜达等将出席。[责编：张倩]</t>
   </si>
   <si>
-    <t>　　新华社华盛顿１２月２日电（记者刘品然　朱东阳）美国总统特朗普１日晚对媒体表示，他或将于明年１月或２月与朝鲜最高领导人金正恩再次举行会晤。
-　　据白宫２日发布的消息，特朗普１日晚从阿根廷乘飞机返回美国途中对媒体说，他与金正恩有着“非常好的关系”，并认为两人或将于明年１月或２月举行会晤。
-　　特朗普表示，目前还没有确定会晤地点，有３个可能的地点正在考虑中。
-　　他还说，会在未来某个时刻邀请金正恩访问美国。
-　　特朗普此前曾表示，他与金正恩的第二次会晤将在今年１１月６日美国中期选举后举行。美国媒体１０月下旬曾援引匿名白宫官员的话报道说，特朗普与金正恩的第二次会晤可能会在明年年初举行。
-　　今年６月，特朗普与金正恩在新加坡会晤并签署联合声明，就“建立新的朝美关系”以及“构建朝鲜半岛持久稳定和平机制”达成一致。[责编：张倩]</t>
-  </si>
-  <si>
     <t>外交部二十国集团事务特使介绍习近平主席出席二十国集团领导人第十三次峰会情况</t>
   </si>
   <si>
@@ -1497,32 +1382,6 @@
   </si>
   <si>
     <t>万豪旗下酒店预订系统遭入侵 股价受影响大幅下挫</t>
-  </si>
-  <si>
-    <t>2018-12-02 15:03</t>
-  </si>
-  <si>
-    <t>　　国际知名酒店集团万豪国际11月30日证实，旗下喜达屋酒店预订系统2014年起遭网络“黑客”入侵，泄露大约5亿客户的个人信息。
-　　美国5个州的总检察长和英国信息专员办公室说，将调查这起网络安全事件。
-　　【波及5亿客户】
-　　万豪国际11月30日说，集团内部安全工具9月8日警告，提醒喜达屋酒店预订系统遭入侵。万豪随即联系网络安全专家，以确认情况。
-　　经调查，万豪确认喜达屋酒店预订系统自2014年起遭黑客侵入。黑客复制并加密一些数据，分步“迁移”复制。万豪9月18日解密这些数据，确认数据源于喜达屋酒店预订系统。
-　　万豪估计，大约5亿曾在喜达屋系统预订酒店的客户受影响。这一系统管理W酒店、瑞吉、希尔顿、威斯汀等知名品牌酒店的客户预定。
-　　其中大约三分之二、即3.27亿客户的姓名、住址、电话号码、电子邮件地址、护照号码以及喜达屋贵宾卡包含的出生日期、性别、预订时间等信息遭泄露；另有一些客户的支付信息遭泄露，包括预订酒店所用信用卡卡号及有效期。
-　　万豪国际发言人杰夫·弗莱赫蒂11月30日说，集团没有完全确认黑客所复制的信息。
-　　美国前联邦网络安全检察官马克·拉谢说：“受影响的人数、数据的私密性以及延迟发现系统遭黑客入侵等因素使这起网络安全事件性质严重。”
-　　美国信用卡网站分析师特德·罗斯曼说，非支付信息遭泄露更应引起注意，犯罪分子可能利用这些信息以客户名义开设虚假账户。
-　　一些客户经由社交媒体“推特”抱怨，使用“上当”“生气”“灾难”等词汇表达不满。一些客户指认万豪“疏忽”，构成“欺诈及不公平商业行为”，要求补偿个人信息遭泄露所致损失。
-　　【系统整合不顺】
-　　万豪国际首席执行官阿恩·索伦森在一份声明中向客户致歉。“我们没有达到客户的要求以及对自己的预期，”索伦森说，“我们正尽一切可能支持客户并将吸取教训，以便更好地发展。”
-　　这家酒店集团为处理这起事件设立专项客户服务电话，从11月30日开始逐一通知可能受影响的客户。
-　　美国康涅狄格、伊利诺伊、马萨诸塞、纽约、宾夕法尼亚5个州的总检察长着手调查这起安全事件。美国联邦调查局说，调查正在推进。英国信息专员办公室作出相同回应。
-　　万豪国际总部位于美国马里兰州蒙哥马利县贝塞斯达，旗下运营的酒店超过6700处，遍及全球，主要分布在北美地区。万豪2015年宣布收购喜达屋酒店及度假村国际集团时，后者拥有2100万忠实客户。这项收购次年完成。
-　　美联社报道，万豪收购喜达屋后，两套酒店预订系统整合过程不顺。一些客户反映系统故障不少：他们的账户积分“无故失踪”、刷信用卡消费获赠免费在酒店住宿的天数不再显示。
-　　按照索伦森的说法，两套系统的整合还没有完成，万豪正寻求逐步淘汰喜达屋酒店预订系统。
-　　受这一事件影响，万豪的股票价格当天大幅下挫。这一酒店集团说，暂时无法估计黑客入侵给集团造成的损失。从长远看，不会影响集团的财务状况。
-　　英国贝尔德股权研究公司推断，黑客入侵喜达屋酒店预订系统产生的关联费用，包括律师费、新增技术和网络安全成本将迫使万豪推迟原定2019年初推广的“忠实客户计划”。（包雪琳）（新华社专特稿）
-[责编：杨煜]</t>
   </si>
   <si>
     <t>美阿拉斯加州强震后现650次余震 暂无重大伤亡</t>
@@ -2246,10 +2105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,19 +2118,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -2285,18 +2144,18 @@
         <v>100000</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5">
         <f ca="1">RANDBETWEEN(1,500)</f>
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="E2" s="5">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
@@ -2310,18 +2169,18 @@
         <v>100001</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D66" ca="1" si="0">RANDBETWEEN(1,500)</f>
-        <v>347</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>304</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E66" ca="1" si="1">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>6</v>
@@ -2335,18 +2194,18 @@
         <v>100002</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>136</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>387</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
@@ -2360,18 +2219,18 @@
         <v>100003</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>447</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>439</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -2385,18 +2244,18 @@
         <v>100004</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>21</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -2410,18 +2269,18 @@
         <v>100005</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>82</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
@@ -2435,18 +2294,18 @@
         <v>100006</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>134</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>198</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>21</v>
@@ -2460,18 +2319,18 @@
         <v>100007</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>440</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>340</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
@@ -2485,18 +2344,18 @@
         <v>100008</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>339</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>27</v>
@@ -2510,18 +2369,18 @@
         <v>100009</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>497</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>242</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>30</v>
@@ -2535,18 +2394,18 @@
         <v>100010</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>434</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>33</v>
@@ -2560,18 +2419,18 @@
         <v>100011</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>366</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>36</v>
@@ -2585,18 +2444,18 @@
         <v>100012</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>473</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>38</v>
@@ -2610,18 +2469,18 @@
         <v>100013</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>313</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>450</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>41</v>
@@ -2635,18 +2494,18 @@
         <v>100014</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>286</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>366</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>44</v>
@@ -2660,18 +2519,18 @@
         <v>100015</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>302</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>26</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>47</v>
@@ -2685,18 +2544,18 @@
         <v>100016</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>227</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>50</v>
@@ -2710,18 +2569,18 @@
         <v>100017</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>213</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>152</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>53</v>
@@ -2735,18 +2594,18 @@
         <v>100018</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>447</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>469</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>56</v>
@@ -2760,18 +2619,18 @@
         <v>100019</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>306</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>404</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>59</v>
@@ -2785,18 +2644,18 @@
         <v>100020</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>392</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>483</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>26</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>62</v>
@@ -2810,18 +2669,18 @@
         <v>100021</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>417</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>31</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>12</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>65</v>
@@ -2835,18 +2694,18 @@
         <v>100022</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>204</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>68</v>
@@ -2860,18 +2719,18 @@
         <v>100023</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>220</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>21</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>71</v>
@@ -2885,18 +2744,18 @@
         <v>100024</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>372</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>488</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>74</v>
@@ -2910,18 +2769,18 @@
         <v>100025</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>453</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>315</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>20</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>77</v>
@@ -2935,18 +2794,18 @@
         <v>100026</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>300</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>333</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>29</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>80</v>
@@ -2960,24 +2819,24 @@
         <v>100027</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>383</v>
+      </c>
+      <c r="E29" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>11</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>419</v>
-      </c>
-      <c r="E29" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2985,24 +2844,24 @@
         <v>100028</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>27</v>
+      </c>
+      <c r="E30" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>24</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>317</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="G30" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3010,24 +2869,24 @@
         <v>100029</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>391</v>
+      </c>
+      <c r="E31" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>3</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="E31" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,24 +2894,24 @@
         <v>100030</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>89</v>
+      </c>
+      <c r="E32" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>29</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>222</v>
-      </c>
-      <c r="E32" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="G32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3060,24 +2919,24 @@
         <v>100031</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="G33" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3085,24 +2944,24 @@
         <v>100032</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
         <v>99</v>
       </c>
-      <c r="D34" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>460</v>
-      </c>
       <c r="E34" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>26</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3110,24 +2969,24 @@
         <v>100033</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>165</v>
+      </c>
+      <c r="E35" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>10</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>428</v>
-      </c>
-      <c r="E35" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="G35" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3135,24 +2994,24 @@
         <v>100034</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>62</v>
+      </c>
+      <c r="E36" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>11</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>486</v>
-      </c>
-      <c r="E36" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="G36" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3160,24 +3019,24 @@
         <v>100035</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>232</v>
+      </c>
+      <c r="E37" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>241</v>
-      </c>
-      <c r="E37" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="G37" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3185,24 +3044,24 @@
         <v>100036</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>104</v>
+      </c>
+      <c r="E38" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>24</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>306</v>
-      </c>
-      <c r="E38" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="G38" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3210,21 +3069,21 @@
         <v>100037</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>114</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>436</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>16</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>14</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>115</v>
@@ -3235,24 +3094,24 @@
         <v>100038</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>472</v>
+      </c>
+      <c r="E40" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>24</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="E40" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3260,24 +3119,24 @@
         <v>100039</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>116</v>
+      </c>
+      <c r="E41" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>24</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="E41" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="G41" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3285,24 +3144,24 @@
         <v>100040</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>38</v>
+      </c>
+      <c r="E42" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>30</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>195</v>
-      </c>
-      <c r="E42" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3310,24 +3169,24 @@
         <v>100041</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>124</v>
+      </c>
+      <c r="E43" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>14</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>417</v>
-      </c>
-      <c r="E43" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="G43" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3335,24 +3194,24 @@
         <v>100042</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>5</v>
+      </c>
+      <c r="E44" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>17</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>232</v>
-      </c>
-      <c r="E44" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3360,24 +3219,24 @@
         <v>100043</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>61</v>
+      </c>
+      <c r="E45" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>29</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D45" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>376</v>
-      </c>
-      <c r="E45" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3385,24 +3244,24 @@
         <v>100044</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>373</v>
+      </c>
+      <c r="E46" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>14</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>316</v>
-      </c>
-      <c r="E46" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3410,24 +3269,24 @@
         <v>100045</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>293</v>
+      </c>
+      <c r="E47" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>16</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D47" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="E47" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3435,24 +3294,24 @@
         <v>100046</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>242</v>
+      </c>
+      <c r="E48" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D48" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>353</v>
-      </c>
-      <c r="E48" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3460,24 +3319,24 @@
         <v>100047</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>198</v>
+      </c>
+      <c r="E49" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>29</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D49" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>275</v>
-      </c>
-      <c r="E49" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="G49" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3485,24 +3344,24 @@
         <v>100048</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>229</v>
+      </c>
+      <c r="E50" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>8</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D50" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>355</v>
-      </c>
-      <c r="E50" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G50" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3510,24 +3369,24 @@
         <v>100049</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>298</v>
+      </c>
+      <c r="E51" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>17</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>352</v>
-      </c>
-      <c r="E51" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="G51" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3535,24 +3394,24 @@
         <v>100050</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>399</v>
+      </c>
+      <c r="E52" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D52" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>331</v>
-      </c>
-      <c r="E52" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="G52" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3560,24 +3419,24 @@
         <v>100051</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>233</v>
+      </c>
+      <c r="E53" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>10</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D53" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="E53" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="G53" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3585,24 +3444,24 @@
         <v>100052</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>448</v>
+      </c>
+      <c r="E54" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>2</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D54" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="E54" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="G54" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3610,21 +3469,21 @@
         <v>100053</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>146</v>
+      </c>
+      <c r="E55" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>28</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D55" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>475</v>
-      </c>
-      <c r="E55" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>162</v>
@@ -3635,24 +3494,24 @@
         <v>100054</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D56" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>151</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>437</v>
       </c>
       <c r="E56" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>15</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>163</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3660,21 +3519,21 @@
         <v>100055</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" s="5">
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>215</v>
+      </c>
+      <c r="E57" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="D57" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>132</v>
-      </c>
-      <c r="E57" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>167</v>
@@ -3685,24 +3544,24 @@
         <v>100056</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D58" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>399</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>221</v>
       </c>
       <c r="E58" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>2</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>168</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3710,24 +3569,24 @@
         <v>100057</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D59" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>122</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>273</v>
       </c>
       <c r="E59" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>17</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3735,24 +3594,24 @@
         <v>100058</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D60" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>339</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>57</v>
       </c>
       <c r="E60" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>3</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3760,24 +3619,24 @@
         <v>100059</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D61" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>337</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>384</v>
       </c>
       <c r="E61" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3785,24 +3644,24 @@
         <v>100060</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D62" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>375</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>193</v>
       </c>
       <c r="E62" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>6</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3810,24 +3669,24 @@
         <v>100061</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D63" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>285</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>476</v>
       </c>
       <c r="E63" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>16</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3835,24 +3694,24 @@
         <v>100062</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>353</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>176</v>
       </c>
       <c r="E64" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>15</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3860,24 +3719,24 @@
         <v>100063</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D65" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>438</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>305</v>
       </c>
       <c r="E65" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>13</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3885,24 +3744,24 @@
         <v>100064</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D66" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>209</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>102</v>
       </c>
       <c r="E66" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>2</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3910,24 +3769,24 @@
         <v>100065</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D67" s="5">
-        <f t="shared" ref="D67:D104" ca="1" si="2">RANDBETWEEN(1,500)</f>
-        <v>299</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>94</v>
       </c>
       <c r="E67" s="5">
-        <f t="shared" ref="E67:E104" ca="1" si="3">RANDBETWEEN(1,30)</f>
-        <v>27</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>23</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3935,24 +3794,24 @@
         <v>100066</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>297</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>312</v>
       </c>
       <c r="E68" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>23</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3960,24 +3819,24 @@
         <v>100067</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>496</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>335</v>
       </c>
       <c r="E69" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>5</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3985,24 +3844,24 @@
         <v>100068</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>470</v>
       </c>
       <c r="E70" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>10</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -4010,24 +3869,24 @@
         <v>100069</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D71" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>137</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>186</v>
       </c>
       <c r="E71" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>17</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4035,24 +3894,24 @@
         <v>100070</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D72" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>235</v>
       </c>
       <c r="E72" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>27</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4060,24 +3919,24 @@
         <v>100071</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D73" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>497</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>482</v>
       </c>
       <c r="E73" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>11</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4085,24 +3944,24 @@
         <v>100072</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D74" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>260</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>249</v>
       </c>
       <c r="E74" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4110,24 +3969,24 @@
         <v>100073</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>469</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>141</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>2</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4135,24 +3994,24 @@
         <v>100074</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>292</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>453</v>
       </c>
       <c r="E76" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>15</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4160,24 +4019,24 @@
         <v>100075</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="D77" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>89</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>232</v>
       </c>
       <c r="E77" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>7</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4185,24 +4044,24 @@
         <v>100076</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>394</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>331</v>
       </c>
       <c r="E78" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>6</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4210,24 +4069,24 @@
         <v>100077</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>227</v>
       </c>
       <c r="E79" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>17</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4235,24 +4094,24 @@
         <v>100078</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="D80" s="5">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>199</v>
+      </c>
+      <c r="E80" s="5">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>14</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="E80" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4260,24 +4119,24 @@
         <v>100079</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="D81" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>305</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>17</v>
       </c>
       <c r="E81" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>27</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4285,24 +4144,24 @@
         <v>100080</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="D82" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>26</v>
       </c>
       <c r="E82" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>22</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4310,24 +4169,24 @@
         <v>100081</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="D83" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>221</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>51</v>
       </c>
       <c r="E83" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>23</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4335,24 +4194,24 @@
         <v>100082</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="D84" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>56</v>
       </c>
       <c r="E84" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>14</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4360,24 +4219,24 @@
         <v>100083</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D85" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>243</v>
       </c>
       <c r="E85" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4385,24 +4244,24 @@
         <v>100084</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="D86" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>279</v>
       </c>
       <c r="E86" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>19</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4410,24 +4269,24 @@
         <v>100085</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D87" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>398</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>470</v>
       </c>
       <c r="E87" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>28</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4435,24 +4294,24 @@
         <v>100086</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D88" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>312</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>132</v>
       </c>
       <c r="E88" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>10</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4460,24 +4319,24 @@
         <v>100087</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="D89" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>479</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>299</v>
       </c>
       <c r="E89" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>11</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4485,24 +4344,24 @@
         <v>100088</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>75</v>
       </c>
       <c r="E90" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>22</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4510,24 +4369,24 @@
         <v>100089</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>423</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>369</v>
       </c>
       <c r="E91" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>22</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4535,24 +4394,24 @@
         <v>100090</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D92" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>162</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>392</v>
       </c>
       <c r="E92" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>10</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4560,24 +4419,24 @@
         <v>100091</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>226</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>274</v>
       </c>
       <c r="E93" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>8</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4585,24 +4444,24 @@
         <v>100092</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>291</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>308</v>
       </c>
       <c r="E94" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>13</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4610,24 +4469,24 @@
         <v>100093</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="D95" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>247</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>450</v>
       </c>
       <c r="E95" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>13</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4635,227 +4494,30 @@
         <v>100094</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="D96" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>478</v>
+        <f ca="1">RANDBETWEEN(1,500)</f>
+        <v>284</v>
       </c>
       <c r="E96" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>12</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
-        <v>100095</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D97" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>114</v>
-      </c>
-      <c r="E97" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
-        <v>100096</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D98" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>94</v>
-      </c>
-      <c r="E98" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>100097</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D99" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>149</v>
-      </c>
-      <c r="E99" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="7">
-        <v>100098</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C100" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D100" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>53</v>
-      </c>
-      <c r="E100" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="7">
-        <v>100099</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D101" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>420</v>
-      </c>
-      <c r="E101" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="7">
-        <v>100100</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="D102" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>196</v>
-      </c>
-      <c r="E102" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="7">
-        <v>100101</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D103" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>220</v>
-      </c>
-      <c r="E103" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="7">
-        <v>100102</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D104" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="E104" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>294</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G96">
+    <sortCondition ref="A65"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>